<commit_message>
changes applied for PRP4 and PAS2023
</commit_message>
<xml_diff>
--- a/multiclass_prob.xlsx
+++ b/multiclass_prob.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhysioUser\OneDrive - University College Cork\Monitor\Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E58FFF-0BCC-41A2-9A9A-8CCB72F260E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDF9954-4BCA-4AC9-B557-FCD4ED526D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:O61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,40 +514,40 @@
         <v>1.4031429999999999E-2</v>
       </c>
       <c r="J2">
-        <v>0.76031919999999997</v>
+        <v>0.78233414999999995</v>
       </c>
       <c r="K2">
-        <v>0.23281895</v>
+        <v>0.20511045</v>
       </c>
       <c r="L2">
-        <v>6.8618799999999999E-3</v>
+        <v>1.255532E-2</v>
       </c>
       <c r="M2">
-        <v>0.37460290000000002</v>
+        <v>0.31529807999999998</v>
       </c>
       <c r="N2">
-        <v>0.51828945000000004</v>
+        <v>0.5278524</v>
       </c>
       <c r="O2">
-        <v>0.10710762</v>
+        <v>0.15684949000000001</v>
       </c>
       <c r="P2">
-        <v>0.34659547000000002</v>
+        <v>0.52108383000000003</v>
       </c>
       <c r="Q2">
-        <v>0.64930164999999995</v>
+        <v>0.45598369999999999</v>
       </c>
       <c r="R2">
-        <v>4.1028699999999998E-3</v>
+        <v>2.2932500000000001E-2</v>
       </c>
       <c r="S2">
-        <v>0.92031604</v>
+        <v>0.58077650000000003</v>
       </c>
       <c r="T2">
-        <v>7.3937520000000007E-2</v>
+        <v>0.22852691999999999</v>
       </c>
       <c r="U2">
-        <v>5.7464700000000001E-3</v>
+        <v>0.19069654</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -579,40 +579,40 @@
         <v>9.3209799999999995E-3</v>
       </c>
       <c r="J3">
-        <v>0.15655920000000001</v>
+        <v>0.18075332</v>
       </c>
       <c r="K3">
-        <v>0.83378830000000004</v>
+        <v>0.7986664</v>
       </c>
       <c r="L3">
-        <v>9.6525199999999995E-3</v>
+        <v>2.0580359999999999E-2</v>
       </c>
       <c r="M3">
-        <v>0.80850506</v>
+        <v>0.65408485999999999</v>
       </c>
       <c r="N3">
-        <v>0.12802712999999999</v>
+        <v>0.16951942</v>
       </c>
       <c r="O3">
-        <v>6.3467759999999998E-2</v>
+        <v>0.17639571000000001</v>
       </c>
       <c r="P3">
-        <v>0.84507049999999995</v>
+        <v>0.57063439999999999</v>
       </c>
       <c r="Q3">
-        <v>2.7012939999999999E-2</v>
+        <v>8.7718489999999996E-2</v>
       </c>
       <c r="R3">
-        <v>0.12791656000000001</v>
+        <v>0.34164709999999998</v>
       </c>
       <c r="S3">
-        <v>0.59618353999999996</v>
+        <v>0.44118332999999998</v>
       </c>
       <c r="T3">
-        <v>0.20599476999999999</v>
+        <v>0.35157853</v>
       </c>
       <c r="U3">
-        <v>0.19782164999999999</v>
+        <v>0.20723815000000001</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -644,40 +644,40 @@
         <v>1.6045319999999998E-2</v>
       </c>
       <c r="J4">
-        <v>0.43179178000000001</v>
+        <v>0.38078097</v>
       </c>
       <c r="K4">
-        <v>0.56064170000000002</v>
+        <v>0.60347265000000005</v>
       </c>
       <c r="L4">
-        <v>7.5665400000000001E-3</v>
+        <v>1.5746429999999999E-2</v>
       </c>
       <c r="M4">
-        <v>0.18418187</v>
+        <v>0.29245929999999998</v>
       </c>
       <c r="N4">
-        <v>0.80151660000000002</v>
+        <v>0.48588544</v>
       </c>
       <c r="O4">
-        <v>1.430153E-2</v>
+        <v>0.22165530999999999</v>
       </c>
       <c r="P4">
-        <v>0.17136235999999999</v>
+        <v>0.22798598</v>
       </c>
       <c r="Q4">
-        <v>0.81952274000000003</v>
+        <v>0.74200975999999996</v>
       </c>
       <c r="R4">
-        <v>9.1149600000000001E-3</v>
+        <v>3.0004220000000002E-2</v>
       </c>
       <c r="S4">
-        <v>0.18858841000000001</v>
+        <v>0.32608503</v>
       </c>
       <c r="T4">
-        <v>0.50699669999999997</v>
+        <v>0.37868685000000002</v>
       </c>
       <c r="U4">
-        <v>0.30441492999999997</v>
+        <v>0.29522811999999998</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -709,40 +709,40 @@
         <v>1.685596E-2</v>
       </c>
       <c r="J5">
-        <v>6.4631099999999997E-2</v>
+        <v>9.5943639999999997E-2</v>
       </c>
       <c r="K5">
-        <v>0.91222530000000002</v>
+        <v>0.87286260000000004</v>
       </c>
       <c r="L5">
-        <v>2.3143560000000001E-2</v>
+        <v>3.1193809999999999E-2</v>
       </c>
       <c r="M5">
-        <v>0.10243240000000001</v>
+        <v>0.22517376</v>
       </c>
       <c r="N5">
-        <v>0.88092893000000005</v>
+        <v>0.58907133</v>
       </c>
       <c r="O5">
-        <v>1.6638650000000001E-2</v>
+        <v>0.18575493000000001</v>
       </c>
       <c r="P5">
-        <v>0.16091316999999999</v>
+        <v>0.26230662999999999</v>
       </c>
       <c r="Q5">
-        <v>0.82030550000000002</v>
+        <v>0.70641569999999998</v>
       </c>
       <c r="R5">
-        <v>1.8781320000000001E-2</v>
+        <v>3.1277630000000001E-2</v>
       </c>
       <c r="S5">
-        <v>2.1685690000000001E-2</v>
+        <v>0.16058183000000001</v>
       </c>
       <c r="T5">
-        <v>0.67880660000000004</v>
+        <v>0.49875950000000002</v>
       </c>
       <c r="U5">
-        <v>0.29950769999999999</v>
+        <v>0.34065866</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -774,40 +774,40 @@
         <v>1.128523E-2</v>
       </c>
       <c r="J6">
-        <v>6.9779809999999998E-2</v>
+        <v>0.1045831</v>
       </c>
       <c r="K6">
-        <v>0.90537540000000005</v>
+        <v>0.85533130000000002</v>
       </c>
       <c r="L6">
-        <v>2.484476E-2</v>
+        <v>4.0085589999999997E-2</v>
       </c>
       <c r="M6">
-        <v>0.97727730000000002</v>
+        <v>0.54612947000000001</v>
       </c>
       <c r="N6">
-        <v>9.5446799999999998E-3</v>
+        <v>0.21363984</v>
       </c>
       <c r="O6">
-        <v>1.317807E-2</v>
+        <v>0.24023068</v>
       </c>
       <c r="P6">
-        <v>0.45277476</v>
+        <v>0.41550690000000001</v>
       </c>
       <c r="Q6">
-        <v>0.34356179999999997</v>
+        <v>0.24809934</v>
       </c>
       <c r="R6">
-        <v>0.20366344</v>
+        <v>0.33639376999999998</v>
       </c>
       <c r="S6">
-        <v>6.6052230000000003E-2</v>
+        <v>0.26231409999999999</v>
       </c>
       <c r="T6">
-        <v>0.92577224999999996</v>
+        <v>0.58141549999999997</v>
       </c>
       <c r="U6">
-        <v>8.1755200000000004E-3</v>
+        <v>0.15627044000000001</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -839,40 +839,40 @@
         <v>1.269167E-2</v>
       </c>
       <c r="J7">
-        <v>7.3741689999999999E-2</v>
+        <v>0.10935567</v>
       </c>
       <c r="K7">
-        <v>0.85835165000000002</v>
+        <v>0.81945069999999998</v>
       </c>
       <c r="L7">
-        <v>6.79067E-2</v>
+        <v>7.1193610000000004E-2</v>
       </c>
       <c r="M7">
-        <v>0.14190243</v>
+        <v>0.50917979999999996</v>
       </c>
       <c r="N7">
-        <v>0.76664144000000001</v>
+        <v>0.25305290000000003</v>
       </c>
       <c r="O7">
-        <v>9.1456179999999998E-2</v>
+        <v>0.23776733999999999</v>
       </c>
       <c r="P7">
-        <v>0.40807181999999997</v>
+        <v>0.38257556999999998</v>
       </c>
       <c r="Q7">
-        <v>0.57986426000000002</v>
+        <v>0.57935669999999995</v>
       </c>
       <c r="R7">
-        <v>1.206398E-2</v>
+        <v>3.8067759999999999E-2</v>
       </c>
       <c r="S7">
-        <v>0.52386840000000001</v>
+        <v>0.39482948000000001</v>
       </c>
       <c r="T7">
-        <v>0.46254965999999997</v>
+        <v>0.4015167</v>
       </c>
       <c r="U7">
-        <v>1.358198E-2</v>
+        <v>0.20365380999999999</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -904,40 +904,40 @@
         <v>1.056386E-2</v>
       </c>
       <c r="J8">
-        <v>6.0414290000000002E-2</v>
+        <v>8.7242559999999997E-2</v>
       </c>
       <c r="K8">
-        <v>0.87144089999999996</v>
+        <v>0.8371845</v>
       </c>
       <c r="L8">
-        <v>6.8144819999999995E-2</v>
+        <v>7.5573000000000001E-2</v>
       </c>
       <c r="M8">
-        <v>4.6798979999999997E-2</v>
+        <v>0.22517376</v>
       </c>
       <c r="N8">
-        <v>0.9407449</v>
+        <v>0.58907133</v>
       </c>
       <c r="O8">
-        <v>1.245609E-2</v>
+        <v>0.18575493000000001</v>
       </c>
       <c r="P8">
-        <v>0.22419976999999999</v>
+        <v>0.29256729999999997</v>
       </c>
       <c r="Q8">
-        <v>0.77024543000000001</v>
+        <v>0.68565595000000001</v>
       </c>
       <c r="R8">
-        <v>5.5548100000000003E-3</v>
+        <v>2.1776750000000001E-2</v>
       </c>
       <c r="S8">
-        <v>6.7356289999999999E-2</v>
+        <v>0.23747083999999999</v>
       </c>
       <c r="T8">
-        <v>0.91661793000000003</v>
+        <v>0.56529032999999995</v>
       </c>
       <c r="U8">
-        <v>1.602582E-2</v>
+        <v>0.19723883</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -969,40 +969,40 @@
         <v>3.1722600000000001E-3</v>
       </c>
       <c r="J9">
-        <v>0.12283384999999999</v>
+        <v>0.13899976</v>
       </c>
       <c r="K9">
-        <v>0.86188299999999995</v>
+        <v>0.82578359999999995</v>
       </c>
       <c r="L9">
-        <v>1.5283120000000001E-2</v>
+        <v>3.5216560000000001E-2</v>
       </c>
       <c r="M9">
-        <v>0.93213869999999999</v>
+        <v>0.62677570000000005</v>
       </c>
       <c r="N9">
-        <v>2.5784729999999999E-2</v>
+        <v>0.18688316999999999</v>
       </c>
       <c r="O9">
-        <v>4.2076509999999998E-2</v>
+        <v>0.18634117</v>
       </c>
       <c r="P9">
-        <v>0.36074349999999999</v>
+        <v>0.25094949999999999</v>
       </c>
       <c r="Q9">
-        <v>0.46717972000000002</v>
+        <v>0.51163506999999997</v>
       </c>
       <c r="R9">
-        <v>0.17207675</v>
+        <v>0.23741543000000001</v>
       </c>
       <c r="S9">
-        <v>0.64478314000000003</v>
+        <v>0.46375379999999999</v>
       </c>
       <c r="T9">
-        <v>0.32695945999999998</v>
+        <v>0.35268748</v>
       </c>
       <c r="U9">
-        <v>2.8257419999999998E-2</v>
+        <v>0.18355875999999999</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1034,40 +1034,40 @@
         <v>2.3594199999999999E-2</v>
       </c>
       <c r="J10">
-        <v>0.75026155000000005</v>
+        <v>0.73936427000000005</v>
       </c>
       <c r="K10">
-        <v>0.22131029999999999</v>
+        <v>0.20834522</v>
       </c>
       <c r="L10">
-        <v>2.8428140000000001E-2</v>
+        <v>5.2290509999999998E-2</v>
       </c>
       <c r="M10">
-        <v>0.18133160000000001</v>
+        <v>0.30935279999999998</v>
       </c>
       <c r="N10">
-        <v>0.7995681</v>
+        <v>0.46433210000000003</v>
       </c>
       <c r="O10">
-        <v>1.910032E-2</v>
+        <v>0.22631513</v>
       </c>
       <c r="P10">
-        <v>0.55969579999999997</v>
+        <v>0.46534242999999997</v>
       </c>
       <c r="Q10">
-        <v>0.43317133000000002</v>
+        <v>0.5045809</v>
       </c>
       <c r="R10">
-        <v>7.1329200000000001E-3</v>
+        <v>3.0076680000000001E-2</v>
       </c>
       <c r="S10">
-        <v>0.82518554</v>
+        <v>0.43002970000000001</v>
       </c>
       <c r="T10">
-        <v>0.11884251</v>
+        <v>0.35416710000000001</v>
       </c>
       <c r="U10">
-        <v>5.5971930000000003E-2</v>
+        <v>0.21580324000000001</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1099,40 +1099,40 @@
         <v>0.68813853999999997</v>
       </c>
       <c r="J11">
-        <v>2.620668E-2</v>
+        <v>5.3404979999999998E-2</v>
       </c>
       <c r="K11">
-        <v>0.67070300000000005</v>
+        <v>0.63425670000000001</v>
       </c>
       <c r="L11">
-        <v>0.30309026999999999</v>
+        <v>0.31233832</v>
       </c>
       <c r="M11">
-        <v>7.2156339999999999E-2</v>
+        <v>0.22887722999999999</v>
       </c>
       <c r="N11">
-        <v>0.91731830000000003</v>
+        <v>0.54203570000000001</v>
       </c>
       <c r="O11">
-        <v>1.0525390000000001E-2</v>
+        <v>0.22908704999999999</v>
       </c>
       <c r="P11">
-        <v>0.58615565000000003</v>
+        <v>0.38679059999999998</v>
       </c>
       <c r="Q11">
-        <v>0.38851451999999997</v>
+        <v>0.55204209999999998</v>
       </c>
       <c r="R11">
-        <v>2.5329850000000001E-2</v>
+        <v>6.1167279999999997E-2</v>
       </c>
       <c r="S11">
-        <v>6.9917950000000006E-2</v>
+        <v>0.21831052000000001</v>
       </c>
       <c r="T11">
-        <v>0.90145600000000004</v>
+        <v>0.58025099999999996</v>
       </c>
       <c r="U11">
-        <v>2.8626059999999998E-2</v>
+        <v>0.20143852000000001</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1164,40 +1164,40 @@
         <v>2.8255079999999998E-2</v>
       </c>
       <c r="J12">
-        <v>0.3684867</v>
+        <v>0.36217470000000002</v>
       </c>
       <c r="K12">
-        <v>0.62033296000000004</v>
+        <v>0.61812794000000004</v>
       </c>
       <c r="L12">
-        <v>1.1180310000000001E-2</v>
+        <v>1.9697360000000001E-2</v>
       </c>
       <c r="M12">
-        <v>0.15583896999999999</v>
+        <v>0.22896089</v>
       </c>
       <c r="N12">
-        <v>0.81467409999999996</v>
+        <v>0.5821577</v>
       </c>
       <c r="O12">
-        <v>2.94869E-2</v>
+        <v>0.18888141</v>
       </c>
       <c r="P12">
-        <v>0.12675864000000001</v>
+        <v>0.19232506999999999</v>
       </c>
       <c r="Q12">
-        <v>0.87043417000000001</v>
+        <v>0.77814150000000004</v>
       </c>
       <c r="R12">
-        <v>2.8072000000000001E-3</v>
+        <v>2.953341E-2</v>
       </c>
       <c r="S12">
-        <v>5.04924E-3</v>
+        <v>0.13979133999999999</v>
       </c>
       <c r="T12">
-        <v>0.8644231</v>
+        <v>0.42468990000000001</v>
       </c>
       <c r="U12">
-        <v>0.13052765999999999</v>
+        <v>0.43551879999999998</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1229,40 +1229,40 @@
         <v>3.627739E-2</v>
       </c>
       <c r="J13">
-        <v>9.1997629999999997E-2</v>
+        <v>0.14209205</v>
       </c>
       <c r="K13">
-        <v>0.90034895999999998</v>
+        <v>0.84466505000000003</v>
       </c>
       <c r="L13">
-        <v>7.6534400000000001E-3</v>
+        <v>1.3243069999999999E-2</v>
       </c>
       <c r="M13">
-        <v>5.0814100000000001E-2</v>
+        <v>0.21030562</v>
       </c>
       <c r="N13">
-        <v>0.87653965</v>
+        <v>0.57011940000000005</v>
       </c>
       <c r="O13">
-        <v>7.2646290000000002E-2</v>
+        <v>0.21957502000000001</v>
       </c>
       <c r="P13">
-        <v>0.76546144000000005</v>
+        <v>0.55896250000000003</v>
       </c>
       <c r="Q13">
-        <v>0.23086153000000001</v>
+        <v>0.41401523000000001</v>
       </c>
       <c r="R13">
-        <v>3.6769799999999998E-3</v>
+        <v>2.7022239999999999E-2</v>
       </c>
       <c r="S13">
-        <v>9.1146100000000004E-3</v>
+        <v>0.21885442999999999</v>
       </c>
       <c r="T13">
-        <v>0.97548520000000005</v>
+        <v>0.58041690000000001</v>
       </c>
       <c r="U13">
-        <v>1.540015E-2</v>
+        <v>0.20072864000000001</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1294,40 +1294,40 @@
         <v>5.5588739999999998E-2</v>
       </c>
       <c r="J14">
-        <v>0.48675205999999999</v>
+        <v>0.47218146999999999</v>
       </c>
       <c r="K14">
-        <v>0.47514856</v>
+        <v>0.48456033999999998</v>
       </c>
       <c r="L14">
-        <v>3.8099429999999997E-2</v>
+        <v>4.325826E-2</v>
       </c>
       <c r="M14">
-        <v>0.73596079999999997</v>
+        <v>0.55543540000000002</v>
       </c>
       <c r="N14">
-        <v>0.15202362999999999</v>
+        <v>0.21510929000000001</v>
       </c>
       <c r="O14">
-        <v>0.11201558</v>
+        <v>0.22945525</v>
       </c>
       <c r="P14">
-        <v>0.43042325999999997</v>
+        <v>0.35211991999999998</v>
       </c>
       <c r="Q14">
-        <v>0.56260279999999996</v>
+        <v>0.61243890000000001</v>
       </c>
       <c r="R14">
-        <v>6.9739800000000003E-3</v>
+        <v>3.5441149999999998E-2</v>
       </c>
       <c r="S14">
-        <v>0.95062435000000001</v>
+        <v>0.57353639999999995</v>
       </c>
       <c r="T14">
-        <v>4.0639040000000001E-2</v>
+        <v>0.25054737999999999</v>
       </c>
       <c r="U14">
-        <v>8.7365900000000007E-3</v>
+        <v>0.17591619999999999</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1359,40 +1359,40 @@
         <v>0.13267529</v>
       </c>
       <c r="J15">
-        <v>1.075445E-2</v>
+        <v>1.7773580000000001E-2</v>
       </c>
       <c r="K15">
-        <v>0.35897509999999999</v>
+        <v>0.36885107</v>
       </c>
       <c r="L15">
-        <v>0.63027040000000001</v>
+        <v>0.61337536999999998</v>
       </c>
       <c r="M15">
-        <v>0.34365487</v>
+        <v>0.36110720000000002</v>
       </c>
       <c r="N15">
-        <v>0.35761290000000001</v>
+        <v>0.37428289999999997</v>
       </c>
       <c r="O15">
-        <v>0.29873221999999999</v>
+        <v>0.26460990000000001</v>
       </c>
       <c r="P15">
-        <v>0.37305297999999998</v>
+        <v>0.37439620000000001</v>
       </c>
       <c r="Q15">
-        <v>0.48179107999999998</v>
+        <v>0.39082798000000002</v>
       </c>
       <c r="R15">
-        <v>0.14515594000000001</v>
+        <v>0.23477581</v>
       </c>
       <c r="S15">
-        <v>4.868625E-2</v>
+        <v>0.21177322000000001</v>
       </c>
       <c r="T15">
-        <v>0.65959319999999999</v>
+        <v>0.48953098</v>
       </c>
       <c r="U15">
-        <v>0.29172053999999997</v>
+        <v>0.29869583</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -1424,40 +1424,40 @@
         <v>0.14644872</v>
       </c>
       <c r="J16">
-        <v>0.55714980000000003</v>
+        <v>0.55213343999999998</v>
       </c>
       <c r="K16">
-        <v>0.3033844</v>
+        <v>0.27971089999999998</v>
       </c>
       <c r="L16">
-        <v>0.13946575</v>
+        <v>0.16815573</v>
       </c>
       <c r="M16">
-        <v>0.61660767000000005</v>
+        <v>0.41474745000000002</v>
       </c>
       <c r="N16">
-        <v>0.27628067000000001</v>
+        <v>0.26733230000000002</v>
       </c>
       <c r="O16">
-        <v>0.10711169</v>
+        <v>0.31792027</v>
       </c>
       <c r="P16">
-        <v>0.22161458000000001</v>
+        <v>0.2131971</v>
       </c>
       <c r="Q16">
-        <v>0.65319954999999996</v>
+        <v>0.65612459999999995</v>
       </c>
       <c r="R16">
-        <v>0.12518588</v>
+        <v>0.13067827000000001</v>
       </c>
       <c r="S16">
-        <v>0.67260635000000002</v>
+        <v>0.52597194999999997</v>
       </c>
       <c r="T16">
-        <v>0.27895418</v>
+        <v>0.23405682</v>
       </c>
       <c r="U16">
-        <v>4.8439459999999997E-2</v>
+        <v>0.23997125</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -1489,40 +1489,40 @@
         <v>7.8413100000000006E-3</v>
       </c>
       <c r="J17">
-        <v>5.8258749999999998E-2</v>
+        <v>0.11041693</v>
       </c>
       <c r="K17">
-        <v>0.93888735999999995</v>
+        <v>0.87948172999999996</v>
       </c>
       <c r="L17">
-        <v>2.8538999999999999E-3</v>
+        <v>1.010134E-2</v>
       </c>
       <c r="M17">
-        <v>3.3267499999999998E-2</v>
+        <v>0.22517376</v>
       </c>
       <c r="N17">
-        <v>0.95367259999999998</v>
+        <v>0.58907133</v>
       </c>
       <c r="O17">
-        <v>1.3059889999999999E-2</v>
+        <v>0.18575493000000001</v>
       </c>
       <c r="P17">
-        <v>0.69743999999999995</v>
+        <v>0.68055975000000002</v>
       </c>
       <c r="Q17">
-        <v>0.29574220000000001</v>
+        <v>0.28506009999999998</v>
       </c>
       <c r="R17">
-        <v>6.81776E-3</v>
+        <v>3.4380130000000002E-2</v>
       </c>
       <c r="S17">
-        <v>0.65349440000000003</v>
+        <v>0.43984276</v>
       </c>
       <c r="T17">
-        <v>0.32386556</v>
+        <v>0.38366707999999999</v>
       </c>
       <c r="U17">
-        <v>2.2640029999999998E-2</v>
+        <v>0.17649013</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1554,40 +1554,40 @@
         <v>1.847907E-2</v>
       </c>
       <c r="J18">
-        <v>8.4121329999999994E-2</v>
+        <v>0.12549646</v>
       </c>
       <c r="K18">
-        <v>0.88167879999999998</v>
+        <v>0.83549640000000003</v>
       </c>
       <c r="L18">
-        <v>3.4199790000000001E-2</v>
+        <v>3.9007010000000002E-2</v>
       </c>
       <c r="M18">
-        <v>0.27237397000000002</v>
+        <v>0.27403829000000002</v>
       </c>
       <c r="N18">
-        <v>0.66528039999999999</v>
+        <v>0.49989650000000002</v>
       </c>
       <c r="O18">
-        <v>6.2345610000000003E-2</v>
+        <v>0.22606523000000001</v>
       </c>
       <c r="P18">
-        <v>2.1820079999999999E-2</v>
+        <v>0.10710905</v>
       </c>
       <c r="Q18">
-        <v>0.97355579999999997</v>
+        <v>0.86917626999999997</v>
       </c>
       <c r="R18">
-        <v>4.6241199999999998E-3</v>
+        <v>2.371471E-2</v>
       </c>
       <c r="S18">
-        <v>8.5788249999999996E-2</v>
+        <v>0.28393844000000001</v>
       </c>
       <c r="T18">
-        <v>0.90759769999999995</v>
+        <v>0.49523240000000002</v>
       </c>
       <c r="U18">
-        <v>6.6139900000000001E-3</v>
+        <v>0.22082913000000001</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -1619,40 +1619,40 @@
         <v>5.7279200000000002E-2</v>
       </c>
       <c r="J19">
-        <v>0.71071035000000005</v>
+        <v>0.69867489999999999</v>
       </c>
       <c r="K19">
-        <v>0.27040550000000002</v>
+        <v>0.25418132999999998</v>
       </c>
       <c r="L19">
-        <v>1.8884120000000001E-2</v>
+        <v>4.7143789999999998E-2</v>
       </c>
       <c r="M19">
-        <v>0.96236926</v>
+        <v>0.58780080000000001</v>
       </c>
       <c r="N19">
-        <v>2.465322E-2</v>
+        <v>0.21540059</v>
       </c>
       <c r="O19">
-        <v>1.2977499999999999E-2</v>
+        <v>0.19679864</v>
       </c>
       <c r="P19">
-        <v>0.96177995000000005</v>
+        <v>0.8351672</v>
       </c>
       <c r="Q19">
-        <v>3.6436070000000001E-2</v>
+        <v>0.15179846999999999</v>
       </c>
       <c r="R19">
-        <v>1.7839399999999999E-3</v>
+        <v>1.303429E-2</v>
       </c>
       <c r="S19">
-        <v>0.97289680000000001</v>
+        <v>0.58703499999999997</v>
       </c>
       <c r="T19">
-        <v>2.2591130000000001E-2</v>
+        <v>0.22649983000000001</v>
       </c>
       <c r="U19">
-        <v>4.5120300000000002E-3</v>
+        <v>0.18646515999999999</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1684,40 +1684,40 @@
         <v>8.3593609999999999E-2</v>
       </c>
       <c r="J20">
-        <v>0.23401607999999999</v>
+        <v>0.24233446</v>
       </c>
       <c r="K20">
-        <v>0.63240176000000003</v>
+        <v>0.60304990000000003</v>
       </c>
       <c r="L20">
-        <v>0.13358212999999999</v>
+        <v>0.1546158</v>
       </c>
       <c r="M20">
-        <v>0.72450490000000001</v>
+        <v>0.38733279999999998</v>
       </c>
       <c r="N20">
-        <v>0.22316200999999999</v>
+        <v>0.44024625000000001</v>
       </c>
       <c r="O20">
-        <v>5.2333119999999997E-2</v>
+        <v>0.17242094999999999</v>
       </c>
       <c r="P20">
-        <v>0.97386799999999996</v>
+        <v>0.84069495999999999</v>
       </c>
       <c r="Q20">
-        <v>3.6253399999999999E-3</v>
+        <v>3.3853000000000001E-2</v>
       </c>
       <c r="R20">
-        <v>2.2506680000000001E-2</v>
+        <v>0.12545201</v>
       </c>
       <c r="S20">
-        <v>0.95516000000000001</v>
+        <v>0.57145290000000004</v>
       </c>
       <c r="T20">
-        <v>4.2240769999999997E-2</v>
+        <v>0.23696268000000001</v>
       </c>
       <c r="U20">
-        <v>2.59918E-3</v>
+        <v>0.19158443999999999</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -1749,40 +1749,40 @@
         <v>1.2760469999999999E-2</v>
       </c>
       <c r="J21">
-        <v>0.70689267</v>
+        <v>0.65966444999999996</v>
       </c>
       <c r="K21">
-        <v>0.24785502000000001</v>
+        <v>0.27132709999999999</v>
       </c>
       <c r="L21">
-        <v>4.5252349999999997E-2</v>
+        <v>6.9008429999999996E-2</v>
       </c>
       <c r="M21">
-        <v>0.67971329999999996</v>
+        <v>0.42735440000000002</v>
       </c>
       <c r="N21">
-        <v>0.26058315999999998</v>
+        <v>0.30645879999999998</v>
       </c>
       <c r="O21">
-        <v>5.9703529999999998E-2</v>
+        <v>0.26618677000000002</v>
       </c>
       <c r="P21">
-        <v>0.93809200000000004</v>
+        <v>0.74247324000000003</v>
       </c>
       <c r="Q21">
-        <v>5.5898009999999998E-2</v>
+        <v>0.22158456000000001</v>
       </c>
       <c r="R21">
-        <v>6.0099899999999998E-3</v>
+        <v>3.5942250000000002E-2</v>
       </c>
       <c r="S21">
-        <v>0.74395869999999997</v>
+        <v>0.47960027999999999</v>
       </c>
       <c r="T21">
-        <v>0.25299572999999997</v>
+        <v>0.33378404</v>
       </c>
       <c r="U21">
-        <v>3.0455600000000001E-3</v>
+        <v>0.18661565999999999</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -1814,40 +1814,40 @@
         <v>0.19813886</v>
       </c>
       <c r="J22">
-        <v>1.6069839999999998E-2</v>
+        <v>3.8462589999999998E-2</v>
       </c>
       <c r="K22">
-        <v>0.9196105</v>
+        <v>0.89974019999999999</v>
       </c>
       <c r="L22">
-        <v>6.4319630000000003E-2</v>
+        <v>6.179722E-2</v>
       </c>
       <c r="M22">
-        <v>0.97598580000000001</v>
+        <v>0.57133657000000004</v>
       </c>
       <c r="N22">
-        <v>1.8859669999999999E-2</v>
+        <v>0.28600736999999998</v>
       </c>
       <c r="O22">
-        <v>5.15454E-3</v>
+        <v>0.14265604000000001</v>
       </c>
       <c r="P22">
-        <v>0.13206322000000001</v>
+        <v>0.18387788999999999</v>
       </c>
       <c r="Q22">
-        <v>0.83651423000000003</v>
+        <v>0.72310509999999995</v>
       </c>
       <c r="R22">
-        <v>3.1422539999999999E-2</v>
+        <v>9.3017089999999997E-2</v>
       </c>
       <c r="S22">
-        <v>2.4669099999999999E-2</v>
+        <v>0.20098316999999999</v>
       </c>
       <c r="T22">
-        <v>0.95294749999999995</v>
+        <v>0.59681799999999996</v>
       </c>
       <c r="U22">
-        <v>2.2383409999999999E-2</v>
+        <v>0.20219892</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -1879,40 +1879,40 @@
         <v>1.8340800000000001E-2</v>
       </c>
       <c r="J23">
-        <v>0.55367580000000005</v>
+        <v>0.50567704000000002</v>
       </c>
       <c r="K23">
-        <v>0.44520777</v>
+        <v>0.48791695000000002</v>
       </c>
       <c r="L23">
-        <v>1.1164300000000001E-3</v>
+        <v>6.4059900000000003E-3</v>
       </c>
       <c r="M23">
-        <v>0.96490909999999996</v>
+        <v>0.64132016999999997</v>
       </c>
       <c r="N23">
-        <v>1.8387179999999999E-2</v>
+        <v>0.19019949999999999</v>
       </c>
       <c r="O23">
-        <v>1.6703719999999998E-2</v>
+        <v>0.16848038000000001</v>
       </c>
       <c r="P23">
-        <v>0.52593429999999997</v>
+        <v>0.74665826999999996</v>
       </c>
       <c r="Q23">
-        <v>0.43272769999999999</v>
+        <v>0.18384797999999999</v>
       </c>
       <c r="R23">
-        <v>4.1337989999999998E-2</v>
+        <v>6.9493769999999996E-2</v>
       </c>
       <c r="S23">
-        <v>0.77248530000000004</v>
+        <v>0.50291735000000004</v>
       </c>
       <c r="T23">
-        <v>0.19509267999999999</v>
+        <v>0.29110399999999997</v>
       </c>
       <c r="U23">
-        <v>3.2421989999999998E-2</v>
+        <v>0.20597866000000001</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -1944,40 +1944,40 @@
         <v>8.7457569999999998E-2</v>
       </c>
       <c r="J24">
-        <v>0.16261080999999999</v>
+        <v>0.19513567000000001</v>
       </c>
       <c r="K24">
-        <v>0.75044960000000005</v>
+        <v>0.72549324999999998</v>
       </c>
       <c r="L24">
-        <v>8.6939569999999994E-2</v>
+        <v>7.9371090000000005E-2</v>
       </c>
       <c r="M24">
-        <v>0.45429765999999999</v>
+        <v>0.34506720000000002</v>
       </c>
       <c r="N24">
-        <v>0.40184300000000001</v>
+        <v>0.43559082999999998</v>
       </c>
       <c r="O24">
-        <v>0.14385934</v>
+        <v>0.21934192999999999</v>
       </c>
       <c r="P24">
-        <v>0.15480949999999999</v>
+        <v>0.36279303000000002</v>
       </c>
       <c r="Q24">
-        <v>0.53503500000000004</v>
+        <v>0.36757719999999999</v>
       </c>
       <c r="R24">
-        <v>0.31015547999999998</v>
+        <v>0.26962977999999999</v>
       </c>
       <c r="S24">
-        <v>0.18556696</v>
+        <v>0.39265299999999997</v>
       </c>
       <c r="T24">
-        <v>0.71935079999999996</v>
+        <v>0.37426510000000002</v>
       </c>
       <c r="U24">
-        <v>9.508221E-2</v>
+        <v>0.23308189000000001</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -2009,40 +2009,40 @@
         <v>0.1016174</v>
       </c>
       <c r="J25">
-        <v>8.8051039999999997E-2</v>
+        <v>0.11909114</v>
       </c>
       <c r="K25">
-        <v>0.89986270000000002</v>
+        <v>0.86874269999999998</v>
       </c>
       <c r="L25">
-        <v>1.2086390000000001E-2</v>
+        <v>1.2166150000000001E-2</v>
       </c>
       <c r="M25">
-        <v>6.7541069999999995E-2</v>
+        <v>0.1641108</v>
       </c>
       <c r="N25">
-        <v>0.85461383999999996</v>
+        <v>0.50934696000000002</v>
       </c>
       <c r="O25">
-        <v>7.7845129999999998E-2</v>
+        <v>0.32654222999999999</v>
       </c>
       <c r="P25">
-        <v>0.11155708</v>
+        <v>0.17051363999999999</v>
       </c>
       <c r="Q25">
-        <v>0.52944446000000001</v>
+        <v>0.4893998</v>
       </c>
       <c r="R25">
-        <v>0.35899841999999998</v>
+        <v>0.34008654999999999</v>
       </c>
       <c r="S25">
-        <v>0.11242399</v>
+        <v>0.23258983</v>
       </c>
       <c r="T25">
-        <v>0.13929036</v>
+        <v>0.24842676999999999</v>
       </c>
       <c r="U25">
-        <v>0.74828565000000002</v>
+        <v>0.51898350000000004</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -2074,40 +2074,40 @@
         <v>2.38821E-2</v>
       </c>
       <c r="J26">
-        <v>0.2748932</v>
+        <v>0.30455458000000002</v>
       </c>
       <c r="K26">
-        <v>0.62014539999999996</v>
+        <v>0.60884879999999997</v>
       </c>
       <c r="L26">
-        <v>0.10496137</v>
+        <v>8.6596610000000004E-2</v>
       </c>
       <c r="M26">
-        <v>8.6531590000000005E-2</v>
+        <v>0.35861187999999999</v>
       </c>
       <c r="N26">
-        <v>0.7939872</v>
+        <v>0.41371983000000001</v>
       </c>
       <c r="O26">
-        <v>0.11948121</v>
+        <v>0.22766834</v>
       </c>
       <c r="P26">
-        <v>2.826381E-2</v>
+        <v>0.11157916</v>
       </c>
       <c r="Q26">
-        <v>0.77111640000000004</v>
+        <v>0.66456556</v>
       </c>
       <c r="R26">
-        <v>0.20061982</v>
+        <v>0.22385527</v>
       </c>
       <c r="S26">
-        <v>0.38814732000000002</v>
+        <v>0.40206419999999998</v>
       </c>
       <c r="T26">
-        <v>0.57278174000000004</v>
+        <v>0.39845574</v>
       </c>
       <c r="U26">
-        <v>3.9070920000000002E-2</v>
+        <v>0.19948004</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -2139,40 +2139,40 @@
         <v>5.7417500000000003E-3</v>
       </c>
       <c r="J27">
-        <v>0.12864101</v>
+        <v>0.16643424000000001</v>
       </c>
       <c r="K27">
-        <v>0.86931186999999999</v>
+        <v>0.82681890000000002</v>
       </c>
       <c r="L27">
-        <v>2.0471700000000001E-3</v>
+        <v>6.7467999999999998E-3</v>
       </c>
       <c r="M27">
-        <v>0.62406830000000002</v>
+        <v>0.29928565000000001</v>
       </c>
       <c r="N27">
-        <v>6.241054E-2</v>
+        <v>0.27862940000000003</v>
       </c>
       <c r="O27">
-        <v>0.31352115000000003</v>
+        <v>0.42208499999999999</v>
       </c>
       <c r="P27">
-        <v>0.93326189999999998</v>
+        <v>0.85333239999999999</v>
       </c>
       <c r="Q27">
-        <v>3.53995E-2</v>
+        <v>8.8359649999999998E-2</v>
       </c>
       <c r="R27">
-        <v>3.133859E-2</v>
+        <v>5.8307949999999997E-2</v>
       </c>
       <c r="S27">
-        <v>0.76033205000000004</v>
+        <v>0.49178233999999998</v>
       </c>
       <c r="T27">
-        <v>0.21574375000000001</v>
+        <v>0.33512753000000001</v>
       </c>
       <c r="U27">
-        <v>2.3924190000000001E-2</v>
+        <v>0.17309015999999999</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -2204,40 +2204,40 @@
         <v>3.9123539999999998E-2</v>
       </c>
       <c r="J28">
-        <v>6.1918920000000002E-2</v>
+        <v>8.5437100000000002E-2</v>
       </c>
       <c r="K28">
-        <v>0.58741129999999997</v>
+        <v>0.60524814999999998</v>
       </c>
       <c r="L28">
-        <v>0.35066967999999998</v>
+        <v>0.30931481999999999</v>
       </c>
       <c r="M28">
-        <v>0.79832329999999996</v>
+        <v>0.51512159999999996</v>
       </c>
       <c r="N28">
-        <v>8.5693400000000003E-2</v>
+        <v>0.25130117000000002</v>
       </c>
       <c r="O28">
-        <v>0.11598333</v>
+        <v>0.23357723999999999</v>
       </c>
       <c r="P28">
-        <v>0.13375089000000001</v>
+        <v>0.24798534999999999</v>
       </c>
       <c r="Q28">
-        <v>0.69672920000000005</v>
+        <v>0.62422529999999998</v>
       </c>
       <c r="R28">
-        <v>0.16951999000000001</v>
+        <v>0.12778935999999999</v>
       </c>
       <c r="S28">
-        <v>0.86587910000000001</v>
+        <v>0.52235699999999996</v>
       </c>
       <c r="T28">
-        <v>7.7939079999999994E-2</v>
+        <v>0.27823471999999999</v>
       </c>
       <c r="U28">
-        <v>5.6181790000000002E-2</v>
+        <v>0.19940833999999999</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -2269,40 +2269,40 @@
         <v>0.14634440000000001</v>
       </c>
       <c r="J29">
-        <v>0.10669155</v>
+        <v>0.12353330999999999</v>
       </c>
       <c r="K29">
-        <v>0.58478629999999998</v>
+        <v>0.56790249999999998</v>
       </c>
       <c r="L29">
-        <v>0.30852214</v>
+        <v>0.30856415999999998</v>
       </c>
       <c r="M29">
-        <v>0.46877229999999998</v>
+        <v>0.35348334999999997</v>
       </c>
       <c r="N29">
-        <v>0.28925243</v>
+        <v>0.37874920000000001</v>
       </c>
       <c r="O29">
-        <v>0.24197531999999999</v>
+        <v>0.26776746000000001</v>
       </c>
       <c r="P29">
-        <v>0.67814976000000005</v>
+        <v>0.52893449999999997</v>
       </c>
       <c r="Q29">
-        <v>0.31617567000000002</v>
+        <v>0.44908234000000002</v>
       </c>
       <c r="R29">
-        <v>5.6745700000000003E-3</v>
+        <v>2.1983200000000001E-2</v>
       </c>
       <c r="S29">
-        <v>0.31607273000000002</v>
+        <v>0.29444182000000002</v>
       </c>
       <c r="T29">
-        <v>0.6259226</v>
+        <v>0.44910902000000003</v>
       </c>
       <c r="U29">
-        <v>5.8004710000000001E-2</v>
+        <v>0.25644913000000003</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -2334,40 +2334,40 @@
         <v>1.527738E-2</v>
       </c>
       <c r="J30">
-        <v>0.17988488</v>
+        <v>0.21167032</v>
       </c>
       <c r="K30">
-        <v>0.80849919999999997</v>
+        <v>0.75836199999999998</v>
       </c>
       <c r="L30">
-        <v>1.161597E-2</v>
+        <v>2.99677E-2</v>
       </c>
       <c r="M30">
-        <v>0.41314355000000003</v>
+        <v>0.39214933000000002</v>
       </c>
       <c r="N30">
-        <v>0.52512186999999999</v>
+        <v>0.35845949999999999</v>
       </c>
       <c r="O30">
-        <v>6.1734579999999997E-2</v>
+        <v>0.24939117999999999</v>
       </c>
       <c r="P30">
-        <v>0.39494394999999999</v>
+        <v>0.29644194000000001</v>
       </c>
       <c r="Q30">
-        <v>0.59566026999999999</v>
+        <v>0.67515650000000005</v>
       </c>
       <c r="R30">
-        <v>9.3958099999999992E-3</v>
+        <v>2.8401570000000001E-2</v>
       </c>
       <c r="S30">
-        <v>0.98250150000000003</v>
+        <v>0.63540730000000001</v>
       </c>
       <c r="T30">
-        <v>1.532239E-2</v>
+        <v>0.20118864</v>
       </c>
       <c r="U30">
-        <v>2.1760799999999999E-3</v>
+        <v>0.16340408000000001</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -2399,40 +2399,40 @@
         <v>8.7290300000000005E-3</v>
       </c>
       <c r="J31">
-        <v>0.3447868</v>
+        <v>0.3490355</v>
       </c>
       <c r="K31">
-        <v>0.65071743999999998</v>
+        <v>0.64091485999999998</v>
       </c>
       <c r="L31">
-        <v>4.4957599999999997E-3</v>
+        <v>1.004969E-2</v>
       </c>
       <c r="M31">
-        <v>6.6103930000000005E-2</v>
+        <v>0.19402437</v>
       </c>
       <c r="N31">
-        <v>0.89376323999999996</v>
+        <v>0.59245380000000003</v>
       </c>
       <c r="O31">
-        <v>4.0132809999999998E-2</v>
+        <v>0.21352185000000001</v>
       </c>
       <c r="P31">
-        <v>0.67349460000000005</v>
+        <v>0.425008</v>
       </c>
       <c r="Q31">
-        <v>2.1085679999999999E-2</v>
+        <v>9.3208479999999996E-2</v>
       </c>
       <c r="R31">
-        <v>0.30541976999999998</v>
+        <v>0.48178349999999998</v>
       </c>
       <c r="S31">
-        <v>0.92355036999999995</v>
+        <v>0.5901689</v>
       </c>
       <c r="T31">
-        <v>7.391209E-2</v>
+        <v>0.25206604999999999</v>
       </c>
       <c r="U31">
-        <v>2.5376000000000001E-3</v>
+        <v>0.15776503</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -2464,40 +2464,40 @@
         <v>1.8442859999999998E-2</v>
       </c>
       <c r="J32">
-        <v>0.79602872999999996</v>
+        <v>0.73696225999999998</v>
       </c>
       <c r="K32">
-        <v>0.18075752</v>
+        <v>0.20762178000000001</v>
       </c>
       <c r="L32">
-        <v>2.3213629999999999E-2</v>
+        <v>5.5416E-2</v>
       </c>
       <c r="M32">
-        <v>0.94470989999999999</v>
+        <v>0.62080930000000001</v>
       </c>
       <c r="N32">
-        <v>3.4074E-2</v>
+        <v>0.17893200000000001</v>
       </c>
       <c r="O32">
-        <v>2.1216180000000001E-2</v>
+        <v>0.20025867</v>
       </c>
       <c r="P32">
-        <v>0.99464034999999995</v>
+        <v>0.93279920000000005</v>
       </c>
       <c r="Q32">
-        <v>3.9137E-3</v>
+        <v>5.7862629999999998E-2</v>
       </c>
       <c r="R32">
-        <v>1.4459900000000001E-3</v>
+        <v>9.3381699999999998E-3</v>
       </c>
       <c r="S32">
-        <v>0.98162950000000004</v>
+        <v>0.63178230000000002</v>
       </c>
       <c r="T32">
-        <v>1.553939E-2</v>
+        <v>0.2028209</v>
       </c>
       <c r="U32">
-        <v>2.8311399999999998E-3</v>
+        <v>0.16539681000000001</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -2529,40 +2529,40 @@
         <v>8.1055999999999993E-3</v>
       </c>
       <c r="J33">
-        <v>9.6698430000000002E-2</v>
+        <v>0.12473991</v>
       </c>
       <c r="K33">
-        <v>0.88054809999999994</v>
+        <v>0.85054300000000005</v>
       </c>
       <c r="L33">
-        <v>2.2753249999999999E-2</v>
+        <v>2.4716990000000001E-2</v>
       </c>
       <c r="M33">
-        <v>0.97558075</v>
+        <v>0.64347695999999999</v>
       </c>
       <c r="N33">
-        <v>1.8469360000000001E-2</v>
+        <v>0.18152660000000001</v>
       </c>
       <c r="O33">
-        <v>5.9498700000000003E-3</v>
+        <v>0.17499644</v>
       </c>
       <c r="P33">
-        <v>0.51125410000000004</v>
+        <v>0.52622179999999996</v>
       </c>
       <c r="Q33">
-        <v>0.4768521</v>
+        <v>0.42766609999999999</v>
       </c>
       <c r="R33">
-        <v>1.1893849999999999E-2</v>
+        <v>4.6112130000000001E-2</v>
       </c>
       <c r="S33">
-        <v>0.44944844</v>
+        <v>0.39057766999999999</v>
       </c>
       <c r="T33">
-        <v>0.54633575999999995</v>
+        <v>0.440992</v>
       </c>
       <c r="U33">
-        <v>4.2157699999999998E-3</v>
+        <v>0.16843032999999999</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -2594,40 +2594,40 @@
         <v>4.9589620000000001E-2</v>
       </c>
       <c r="J34">
-        <v>0.31975439999999999</v>
+        <v>0.41036109999999998</v>
       </c>
       <c r="K34">
-        <v>0.58555690000000005</v>
+        <v>0.49737861999999999</v>
       </c>
       <c r="L34">
-        <v>9.4688700000000001E-2</v>
+        <v>9.226028E-2</v>
       </c>
       <c r="M34">
-        <v>0.67372679999999996</v>
+        <v>0.43062958000000001</v>
       </c>
       <c r="N34">
-        <v>0.25487235000000003</v>
+        <v>0.35739989999999999</v>
       </c>
       <c r="O34">
-        <v>7.140088E-2</v>
+        <v>0.21197050000000001</v>
       </c>
       <c r="P34">
-        <v>0.14544029999999999</v>
+        <v>0.20505385000000001</v>
       </c>
       <c r="Q34">
-        <v>0.84048210000000001</v>
+        <v>0.7610595</v>
       </c>
       <c r="R34">
-        <v>1.4077640000000001E-2</v>
+        <v>3.3886600000000003E-2</v>
       </c>
       <c r="S34">
-        <v>0.75249124000000001</v>
+        <v>0.44685352</v>
       </c>
       <c r="T34">
-        <v>7.6725810000000005E-2</v>
+        <v>0.21720336000000001</v>
       </c>
       <c r="U34">
-        <v>0.17078294999999999</v>
+        <v>0.33594307000000001</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -2659,40 +2659,40 @@
         <v>5.0798280000000001E-2</v>
       </c>
       <c r="J35">
-        <v>0.19433278000000001</v>
+        <v>0.22173472</v>
       </c>
       <c r="K35">
-        <v>0.79783665999999998</v>
+        <v>0.76320469999999996</v>
       </c>
       <c r="L35">
-        <v>7.8305200000000005E-3</v>
+        <v>1.506061E-2</v>
       </c>
       <c r="M35">
-        <v>0.2126536</v>
+        <v>0.23814595999999999</v>
       </c>
       <c r="N35">
-        <v>0.70264923999999995</v>
+        <v>0.56598630000000005</v>
       </c>
       <c r="O35">
-        <v>8.4697170000000002E-2</v>
+        <v>0.19586775000000001</v>
       </c>
       <c r="P35">
-        <v>0.61765270000000005</v>
+        <v>0.50611264</v>
       </c>
       <c r="Q35">
-        <v>0.35397434</v>
+        <v>0.44264364</v>
       </c>
       <c r="R35">
-        <v>2.8372919999999999E-2</v>
+        <v>5.1243690000000001E-2</v>
       </c>
       <c r="S35">
-        <v>0.40419719999999998</v>
+        <v>0.30765206</v>
       </c>
       <c r="T35">
-        <v>0.58999840000000003</v>
+        <v>0.50921799999999995</v>
       </c>
       <c r="U35">
-        <v>5.8043399999999998E-3</v>
+        <v>0.18312998</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -2724,40 +2724,40 @@
         <v>2.4846239999999999E-2</v>
       </c>
       <c r="J36">
-        <v>0.64512749999999996</v>
+        <v>0.58734136999999997</v>
       </c>
       <c r="K36">
-        <v>0.32790702999999999</v>
+        <v>0.37736794000000001</v>
       </c>
       <c r="L36">
-        <v>2.696554E-2</v>
+        <v>3.5290630000000003E-2</v>
       </c>
       <c r="M36">
-        <v>0.88407046</v>
+        <v>0.58672064999999995</v>
       </c>
       <c r="N36">
-        <v>3.5850159999999999E-2</v>
+        <v>0.21382213</v>
       </c>
       <c r="O36">
-        <v>8.0079380000000006E-2</v>
+        <v>0.19945726</v>
       </c>
       <c r="P36">
-        <v>0.71091890000000002</v>
+        <v>0.71736489999999997</v>
       </c>
       <c r="Q36">
-        <v>0.21154862999999999</v>
+        <v>0.21917927000000001</v>
       </c>
       <c r="R36">
-        <v>7.7532459999999997E-2</v>
+        <v>6.3455789999999998E-2</v>
       </c>
       <c r="S36">
-        <v>0.41941000000000001</v>
+        <v>0.49652230000000003</v>
       </c>
       <c r="T36">
-        <v>0.57774484000000004</v>
+        <v>0.34737574999999998</v>
       </c>
       <c r="U36">
-        <v>2.8452E-3</v>
+        <v>0.15610191000000001</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -2789,40 +2789,40 @@
         <v>0.10738593</v>
       </c>
       <c r="J37">
-        <v>5.9709690000000003E-2</v>
+        <v>9.024981E-2</v>
       </c>
       <c r="K37">
-        <v>0.93805426000000003</v>
+        <v>0.90366215000000005</v>
       </c>
       <c r="L37">
-        <v>2.2361199999999999E-3</v>
+        <v>6.08824E-3</v>
       </c>
       <c r="M37">
-        <v>0.45930876999999998</v>
+        <v>0.56075419999999998</v>
       </c>
       <c r="N37">
-        <v>0.49565517999999997</v>
+        <v>0.30043130000000001</v>
       </c>
       <c r="O37">
-        <v>4.5036020000000003E-2</v>
+        <v>0.13881452</v>
       </c>
       <c r="P37">
-        <v>0.99461460000000002</v>
+        <v>0.94216509999999998</v>
       </c>
       <c r="Q37">
-        <v>4.2701500000000003E-3</v>
+        <v>4.6362819999999999E-2</v>
       </c>
       <c r="R37">
-        <v>1.1152600000000001E-3</v>
+        <v>1.1472090000000001E-2</v>
       </c>
       <c r="S37">
-        <v>0.98879134999999996</v>
+        <v>0.571793</v>
       </c>
       <c r="T37">
-        <v>9.8690400000000008E-3</v>
+        <v>0.28241724000000001</v>
       </c>
       <c r="U37">
-        <v>1.3395900000000001E-3</v>
+        <v>0.1457898</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -2854,40 +2854,40 @@
         <v>6.8468059999999997E-2</v>
       </c>
       <c r="J38">
-        <v>0.48554682999999998</v>
+        <v>0.46739677000000002</v>
       </c>
       <c r="K38">
-        <v>0.44759557</v>
+        <v>0.47537032000000001</v>
       </c>
       <c r="L38">
-        <v>6.6857570000000005E-2</v>
+        <v>5.7232930000000001E-2</v>
       </c>
       <c r="M38">
-        <v>0.61997910000000001</v>
+        <v>0.4090801</v>
       </c>
       <c r="N38">
-        <v>2.661442E-2</v>
+        <v>0.26922634000000001</v>
       </c>
       <c r="O38">
-        <v>0.35340650000000001</v>
+        <v>0.32169356999999998</v>
       </c>
       <c r="P38">
-        <v>0.16630339999999999</v>
+        <v>0.37088436000000002</v>
       </c>
       <c r="Q38">
-        <v>0.3607746</v>
+        <v>0.19510153</v>
       </c>
       <c r="R38">
-        <v>0.47292202999999999</v>
+        <v>0.43401408000000002</v>
       </c>
       <c r="S38">
-        <v>0.64074299999999995</v>
+        <v>0.45765699999999998</v>
       </c>
       <c r="T38">
-        <v>0.34399091999999998</v>
+        <v>0.35329450000000001</v>
       </c>
       <c r="U38">
-        <v>1.526606E-2</v>
+        <v>0.18904850000000001</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -2919,40 +2919,40 @@
         <v>0.21423890000000001</v>
       </c>
       <c r="J39">
-        <v>0.78970660000000004</v>
+        <v>0.77903820000000001</v>
       </c>
       <c r="K39">
-        <v>0.15111732</v>
+        <v>0.15656022999999999</v>
       </c>
       <c r="L39">
-        <v>5.9176119999999999E-2</v>
+        <v>6.4401570000000005E-2</v>
       </c>
       <c r="M39">
-        <v>0.9327493</v>
+        <v>0.63841903</v>
       </c>
       <c r="N39">
-        <v>3.7693549999999999E-2</v>
+        <v>0.17080575000000001</v>
       </c>
       <c r="O39">
-        <v>2.9557159999999999E-2</v>
+        <v>0.19077516</v>
       </c>
       <c r="P39">
-        <v>0.92276990000000003</v>
+        <v>0.84987897000000001</v>
       </c>
       <c r="Q39">
-        <v>3.7620239999999999E-2</v>
+        <v>9.8819760000000006E-2</v>
       </c>
       <c r="R39">
-        <v>3.9609859999999997E-2</v>
+        <v>5.1301319999999997E-2</v>
       </c>
       <c r="S39">
-        <v>0.96736960000000005</v>
+        <v>0.63232553000000002</v>
       </c>
       <c r="T39">
-        <v>2.9174829999999999E-2</v>
+        <v>0.19240320999999999</v>
       </c>
       <c r="U39">
-        <v>3.4555800000000002E-3</v>
+        <v>0.17527121000000001</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -2984,40 +2984,40 @@
         <v>3.9902079999999999E-2</v>
       </c>
       <c r="J40">
-        <v>0.35561836000000002</v>
+        <v>0.35914800000000002</v>
       </c>
       <c r="K40">
-        <v>0.59230740000000004</v>
+        <v>0.58455760000000001</v>
       </c>
       <c r="L40">
-        <v>5.2074349999999998E-2</v>
+        <v>5.629439E-2</v>
       </c>
       <c r="M40">
-        <v>4.0242180000000002E-2</v>
+        <v>0.19214350999999999</v>
       </c>
       <c r="N40">
-        <v>0.91693765000000005</v>
+        <v>0.61453915000000003</v>
       </c>
       <c r="O40">
-        <v>4.282014E-2</v>
+        <v>0.19331735</v>
       </c>
       <c r="P40">
-        <v>0.49691635000000001</v>
+        <v>0.44586863999999998</v>
       </c>
       <c r="Q40">
-        <v>0.49174615999999999</v>
+        <v>0.51859390000000005</v>
       </c>
       <c r="R40">
-        <v>1.1337470000000001E-2</v>
+        <v>3.553742E-2</v>
       </c>
       <c r="S40">
-        <v>0.31931229999999999</v>
+        <v>0.29229927</v>
       </c>
       <c r="T40">
-        <v>0.56431984999999996</v>
+        <v>0.45128744999999998</v>
       </c>
       <c r="U40">
-        <v>0.11636784999999999</v>
+        <v>0.25641328000000002</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -3049,40 +3049,40 @@
         <v>1.844001E-2</v>
       </c>
       <c r="J41">
-        <v>2.9134879999999998E-2</v>
+        <v>4.4535619999999998E-2</v>
       </c>
       <c r="K41">
-        <v>0.96883350000000001</v>
+        <v>0.94974714999999998</v>
       </c>
       <c r="L41">
-        <v>2.0317099999999999E-3</v>
+        <v>5.7172799999999999E-3</v>
       </c>
       <c r="M41">
-        <v>5.5938200000000002E-3</v>
+        <v>0.17227101</v>
       </c>
       <c r="N41">
-        <v>0.96330804000000003</v>
+        <v>0.64788467000000005</v>
       </c>
       <c r="O41">
-        <v>3.109808E-2</v>
+        <v>0.17984432</v>
       </c>
       <c r="P41">
-        <v>0.90711710000000001</v>
+        <v>0.88462704000000003</v>
       </c>
       <c r="Q41">
-        <v>5.7146919999999997E-2</v>
+        <v>6.5446039999999997E-2</v>
       </c>
       <c r="R41">
-        <v>3.5735910000000003E-2</v>
+        <v>4.9926940000000003E-2</v>
       </c>
       <c r="S41">
-        <v>0.52296609999999999</v>
+        <v>0.34678522000000001</v>
       </c>
       <c r="T41">
-        <v>0.38658347999999998</v>
+        <v>0.44272404999999998</v>
       </c>
       <c r="U41">
-        <v>9.0450459999999996E-2</v>
+        <v>0.21049072999999999</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -3114,40 +3114,40 @@
         <v>2.33417E-3</v>
       </c>
       <c r="J42">
-        <v>0.34463406000000002</v>
+        <v>0.32394410000000001</v>
       </c>
       <c r="K42">
-        <v>0.65370879999999998</v>
+        <v>0.67043079999999999</v>
       </c>
       <c r="L42">
-        <v>1.6570999999999999E-3</v>
+        <v>5.6251499999999998E-3</v>
       </c>
       <c r="M42">
-        <v>0.82895553</v>
+        <v>0.57513714000000005</v>
       </c>
       <c r="N42">
-        <v>5.7757129999999997E-2</v>
+        <v>0.23669090000000001</v>
       </c>
       <c r="O42">
-        <v>0.11328733000000001</v>
+        <v>0.18817200000000001</v>
       </c>
       <c r="P42">
-        <v>0.50210553000000002</v>
+        <v>0.57850754000000004</v>
       </c>
       <c r="Q42">
-        <v>0.49674015999999999</v>
+        <v>0.40917075000000003</v>
       </c>
       <c r="R42">
-        <v>1.15427E-3</v>
+        <v>1.23217E-2</v>
       </c>
       <c r="S42">
-        <v>0.92860030000000005</v>
+        <v>0.60743409999999998</v>
       </c>
       <c r="T42">
-        <v>6.0068009999999998E-2</v>
+        <v>0.2198658</v>
       </c>
       <c r="U42">
-        <v>1.133169E-2</v>
+        <v>0.17270014</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -3179,40 +3179,40 @@
         <v>0.13635021</v>
       </c>
       <c r="J43">
-        <v>4.4491599999999997E-3</v>
+        <v>1.234764E-2</v>
       </c>
       <c r="K43">
-        <v>0.98796534999999996</v>
+        <v>0.97458935000000002</v>
       </c>
       <c r="L43">
-        <v>7.5854299999999998E-3</v>
+        <v>1.306298E-2</v>
       </c>
       <c r="M43">
-        <v>0.83821034000000005</v>
+        <v>0.56446569999999996</v>
       </c>
       <c r="N43">
-        <v>6.0853079999999997E-2</v>
+        <v>0.17074728</v>
       </c>
       <c r="O43">
-        <v>0.10093661</v>
+        <v>0.26478701999999998</v>
       </c>
       <c r="P43">
-        <v>9.6203129999999998E-2</v>
+        <v>0.18392020000000001</v>
       </c>
       <c r="Q43">
-        <v>0.57134174999999998</v>
+        <v>0.60747119999999999</v>
       </c>
       <c r="R43">
-        <v>0.33245507000000002</v>
+        <v>0.20860856999999999</v>
       </c>
       <c r="S43">
-        <v>2.47882E-2</v>
+        <v>0.2334138</v>
       </c>
       <c r="T43">
-        <v>0.86459660000000005</v>
+        <v>0.49437046000000001</v>
       </c>
       <c r="U43">
-        <v>0.11061521000000001</v>
+        <v>0.27221574999999998</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -3244,40 +3244,40 @@
         <v>6.3936839999999995E-2</v>
       </c>
       <c r="J44">
-        <v>0.77564376999999995</v>
+        <v>0.76620566999999995</v>
       </c>
       <c r="K44">
-        <v>0.21961127</v>
+        <v>0.22507893000000001</v>
       </c>
       <c r="L44">
-        <v>4.7450399999999998E-3</v>
+        <v>8.7153100000000004E-3</v>
       </c>
       <c r="M44">
-        <v>0.53079443999999998</v>
+        <v>0.31325087000000001</v>
       </c>
       <c r="N44">
-        <v>0.25711566000000002</v>
+        <v>0.30848697000000003</v>
       </c>
       <c r="O44">
-        <v>0.21208987000000001</v>
+        <v>0.37826219999999999</v>
       </c>
       <c r="P44">
-        <v>0.38708471999999999</v>
+        <v>0.304784</v>
       </c>
       <c r="Q44">
-        <v>0.52944199999999997</v>
+        <v>0.56788576000000002</v>
       </c>
       <c r="R44">
-        <v>8.3473249999999999E-2</v>
+        <v>0.12733026</v>
       </c>
       <c r="S44">
-        <v>4.2666370000000002E-2</v>
+        <v>0.24926138</v>
       </c>
       <c r="T44">
-        <v>0.91200376000000005</v>
+        <v>0.46809392999999999</v>
       </c>
       <c r="U44">
-        <v>4.5329899999999999E-2</v>
+        <v>0.28264470000000003</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
@@ -3309,40 +3309,40 @@
         <v>1.0269759999999999E-2</v>
       </c>
       <c r="J45">
-        <v>0.42937338000000003</v>
+        <v>0.44310105</v>
       </c>
       <c r="K45">
-        <v>0.56836520000000001</v>
+        <v>0.55023230000000001</v>
       </c>
       <c r="L45">
-        <v>2.2614000000000002E-3</v>
+        <v>6.6666700000000004E-3</v>
       </c>
       <c r="M45">
-        <v>0.95928150000000001</v>
+        <v>0.59343489999999999</v>
       </c>
       <c r="N45">
-        <v>2.006488E-2</v>
+        <v>0.18264559</v>
       </c>
       <c r="O45">
-        <v>2.065357E-2</v>
+        <v>0.22391955999999999</v>
       </c>
       <c r="P45">
-        <v>0.95792633000000005</v>
+        <v>0.90955090000000005</v>
       </c>
       <c r="Q45">
-        <v>2.91112E-2</v>
+        <v>5.6179449999999999E-2</v>
       </c>
       <c r="R45">
-        <v>1.296244E-2</v>
+        <v>3.4269649999999999E-2</v>
       </c>
       <c r="S45">
-        <v>0.90176100000000003</v>
+        <v>0.59881293999999996</v>
       </c>
       <c r="T45">
-        <v>9.3217510000000003E-2</v>
+        <v>0.24063182999999999</v>
       </c>
       <c r="U45">
-        <v>5.0214999999999999E-3</v>
+        <v>0.16055523999999999</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -3374,40 +3374,40 @@
         <v>1.8961059999999998E-2</v>
       </c>
       <c r="J46">
-        <v>0.13894498</v>
+        <v>0.200317</v>
       </c>
       <c r="K46">
-        <v>0.85017335000000005</v>
+        <v>0.78280240000000001</v>
       </c>
       <c r="L46">
-        <v>1.0881679999999999E-2</v>
+        <v>1.6880550000000001E-2</v>
       </c>
       <c r="M46">
-        <v>0.95834109999999995</v>
+        <v>0.64270249999999995</v>
       </c>
       <c r="N46">
-        <v>2.6301560000000002E-2</v>
+        <v>0.18698886000000001</v>
       </c>
       <c r="O46">
-        <v>1.535737E-2</v>
+        <v>0.17030862999999999</v>
       </c>
       <c r="P46">
-        <v>0.85236645</v>
+        <v>0.81578810000000002</v>
       </c>
       <c r="Q46">
-        <v>0.11418353000000001</v>
+        <v>0.13121767000000001</v>
       </c>
       <c r="R46">
-        <v>3.3450010000000002E-2</v>
+        <v>5.2994230000000003E-2</v>
       </c>
       <c r="S46">
-        <v>0.78329760000000004</v>
+        <v>0.57345223000000001</v>
       </c>
       <c r="T46">
-        <v>0.21257503</v>
+        <v>0.27851150000000002</v>
       </c>
       <c r="U46">
-        <v>4.1273899999999999E-3</v>
+        <v>0.14803627</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
@@ -3439,40 +3439,40 @@
         <v>3.4302230000000003E-2</v>
       </c>
       <c r="J47">
-        <v>0.39138800000000001</v>
+        <v>0.39605164999999998</v>
       </c>
       <c r="K47">
-        <v>0.51670099999999997</v>
+        <v>0.50579229999999997</v>
       </c>
       <c r="L47">
-        <v>9.1911000000000007E-2</v>
+        <v>9.8156060000000003E-2</v>
       </c>
       <c r="M47">
-        <v>0.84795019999999999</v>
+        <v>0.45709538</v>
       </c>
       <c r="N47">
-        <v>0.12041014999999999</v>
+        <v>0.36209398999999998</v>
       </c>
       <c r="O47">
-        <v>3.1639590000000002E-2</v>
+        <v>0.18081064999999999</v>
       </c>
       <c r="P47">
-        <v>0.12364781</v>
+        <v>0.21960452</v>
       </c>
       <c r="Q47">
-        <v>0.86722577000000001</v>
+        <v>0.74690270000000003</v>
       </c>
       <c r="R47">
-        <v>9.1263899999999998E-3</v>
+        <v>3.3492790000000001E-2</v>
       </c>
       <c r="S47">
-        <v>0.56445533000000003</v>
+        <v>0.34086186000000002</v>
       </c>
       <c r="T47">
-        <v>0.34531604999999999</v>
+        <v>0.44206935000000003</v>
       </c>
       <c r="U47">
-        <v>9.0228600000000006E-2</v>
+        <v>0.21706876</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -3504,40 +3504,40 @@
         <v>6.5261570000000005E-2</v>
       </c>
       <c r="J48">
-        <v>0.71100770000000002</v>
+        <v>0.68862425999999999</v>
       </c>
       <c r="K48">
-        <v>0.19650382</v>
+        <v>0.21345183000000001</v>
       </c>
       <c r="L48">
-        <v>9.2488470000000003E-2</v>
+        <v>9.7923899999999994E-2</v>
       </c>
       <c r="M48">
-        <v>0.98578334000000001</v>
+        <v>0.65263599999999999</v>
       </c>
       <c r="N48">
-        <v>9.7787099999999995E-3</v>
+        <v>0.17591082</v>
       </c>
       <c r="O48">
-        <v>4.4379299999999997E-3</v>
+        <v>0.17145315</v>
       </c>
       <c r="P48">
-        <v>0.99306890000000003</v>
+        <v>0.96834160000000002</v>
       </c>
       <c r="Q48">
-        <v>5.5427799999999998E-3</v>
+        <v>2.3057049999999999E-2</v>
       </c>
       <c r="R48">
-        <v>1.3883599999999999E-3</v>
+        <v>8.6013300000000008E-3</v>
       </c>
       <c r="S48">
-        <v>0.99164516000000003</v>
+        <v>0.64035165000000005</v>
       </c>
       <c r="T48">
-        <v>3.2592799999999998E-3</v>
+        <v>0.19965121</v>
       </c>
       <c r="U48">
-        <v>5.0955899999999997E-3</v>
+        <v>0.15999716999999999</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
@@ -3569,40 +3569,40 @@
         <v>0.12358534</v>
       </c>
       <c r="J49">
-        <v>0.62580630000000004</v>
+        <v>0.60107379999999999</v>
       </c>
       <c r="K49">
-        <v>0.29982969999999998</v>
+        <v>0.30029324000000002</v>
       </c>
       <c r="L49">
-        <v>7.4364029999999998E-2</v>
+        <v>9.8632940000000002E-2</v>
       </c>
       <c r="M49">
-        <v>0.97138599999999997</v>
+        <v>0.65080879999999997</v>
       </c>
       <c r="N49">
-        <v>1.114682E-2</v>
+        <v>0.17488426000000001</v>
       </c>
       <c r="O49">
-        <v>1.7467119999999999E-2</v>
+        <v>0.17430691000000001</v>
       </c>
       <c r="P49">
-        <v>0.98540280000000002</v>
+        <v>0.93630146999999997</v>
       </c>
       <c r="Q49">
-        <v>1.2267109999999999E-2</v>
+        <v>5.3335550000000002E-2</v>
       </c>
       <c r="R49">
-        <v>2.3300899999999999E-3</v>
+        <v>1.0362970000000001E-2</v>
       </c>
       <c r="S49">
-        <v>0.84620136000000001</v>
+        <v>0.53895090000000001</v>
       </c>
       <c r="T49">
-        <v>4.8932110000000001E-2</v>
+        <v>0.25359317999999997</v>
       </c>
       <c r="U49">
-        <v>0.10486653</v>
+        <v>0.20745589</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
@@ -3634,40 +3634,40 @@
         <v>4.8400800000000001E-3</v>
       </c>
       <c r="J50">
-        <v>0.61360824000000003</v>
+        <v>0.62868040000000003</v>
       </c>
       <c r="K50">
-        <v>0.38236234000000002</v>
+        <v>0.36106598000000001</v>
       </c>
       <c r="L50">
-        <v>4.0294199999999997E-3</v>
+        <v>1.025364E-2</v>
       </c>
       <c r="M50">
-        <v>0.97459804999999999</v>
+        <v>0.65080879999999997</v>
       </c>
       <c r="N50">
-        <v>1.0082860000000001E-2</v>
+        <v>0.17488426000000001</v>
       </c>
       <c r="O50">
-        <v>1.531915E-2</v>
+        <v>0.17430691000000001</v>
       </c>
       <c r="P50">
-        <v>0.59554010000000002</v>
+        <v>0.56345699999999999</v>
       </c>
       <c r="Q50">
-        <v>0.38802710000000001</v>
+        <v>0.41129112000000001</v>
       </c>
       <c r="R50">
-        <v>1.6432849999999999E-2</v>
+        <v>2.5251869999999999E-2</v>
       </c>
       <c r="S50">
-        <v>0.92064756000000003</v>
+        <v>0.59760429999999998</v>
       </c>
       <c r="T50">
-        <v>6.230745E-2</v>
+        <v>0.25056899999999999</v>
       </c>
       <c r="U50">
-        <v>1.7044989999999999E-2</v>
+        <v>0.15182671</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
@@ -3699,40 +3699,40 @@
         <v>6.77408E-3</v>
       </c>
       <c r="J51">
-        <v>0.49688196000000001</v>
+        <v>0.50977490000000003</v>
       </c>
       <c r="K51">
-        <v>0.49590139999999999</v>
+        <v>0.47763666999999999</v>
       </c>
       <c r="L51">
-        <v>7.2166399999999999E-3</v>
+        <v>1.258841E-2</v>
       </c>
       <c r="M51">
-        <v>0.84358149999999998</v>
+        <v>0.56131580000000003</v>
       </c>
       <c r="N51">
-        <v>0.14075172999999999</v>
+        <v>0.27164159999999998</v>
       </c>
       <c r="O51">
-        <v>1.5666739999999998E-2</v>
+        <v>0.16704261000000001</v>
       </c>
       <c r="P51">
-        <v>0.86067366999999995</v>
+        <v>0.72395074000000004</v>
       </c>
       <c r="Q51">
-        <v>0.13342656</v>
+        <v>0.23810215000000001</v>
       </c>
       <c r="R51">
-        <v>5.8997900000000002E-3</v>
+        <v>3.7947149999999999E-2</v>
       </c>
       <c r="S51">
-        <v>0.96252846999999997</v>
+        <v>0.63241919999999996</v>
       </c>
       <c r="T51">
-        <v>3.5966310000000001E-2</v>
+        <v>0.20803878000000001</v>
       </c>
       <c r="U51">
-        <v>1.50519E-3</v>
+        <v>0.15954198</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
@@ -3764,40 +3764,40 @@
         <v>0.38688235999999998</v>
       </c>
       <c r="J52">
-        <v>5.7205230000000003E-2</v>
+        <v>6.5291940000000007E-2</v>
       </c>
       <c r="K52">
-        <v>0.93532499999999996</v>
+        <v>0.92276685999999997</v>
       </c>
       <c r="L52">
-        <v>7.4697699999999997E-3</v>
+        <v>1.194129E-2</v>
       </c>
       <c r="M52">
-        <v>0.23358424999999999</v>
+        <v>0.23814595999999999</v>
       </c>
       <c r="N52">
-        <v>0.7184353</v>
+        <v>0.56598630000000005</v>
       </c>
       <c r="O52">
-        <v>4.7980460000000003E-2</v>
+        <v>0.19586775000000001</v>
       </c>
       <c r="P52">
-        <v>5.4575709999999999E-2</v>
+        <v>0.21870007</v>
       </c>
       <c r="Q52">
-        <v>0.94162846</v>
+        <v>0.76589430000000003</v>
       </c>
       <c r="R52">
-        <v>3.7957899999999998E-3</v>
+        <v>1.54056E-2</v>
       </c>
       <c r="S52">
-        <v>0.48454049999999999</v>
+        <v>0.48498422000000002</v>
       </c>
       <c r="T52">
-        <v>0.50074415999999999</v>
+        <v>0.33553460000000002</v>
       </c>
       <c r="U52">
-        <v>1.471536E-2</v>
+        <v>0.17948115000000001</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
@@ -3829,40 +3829,40 @@
         <v>4.9502940000000002E-2</v>
       </c>
       <c r="J53">
-        <v>0.73678460000000001</v>
+        <v>0.68328800000000001</v>
       </c>
       <c r="K53">
-        <v>0.23598044000000001</v>
+        <v>0.27160034</v>
       </c>
       <c r="L53">
-        <v>2.7234899999999999E-2</v>
+        <v>4.5111659999999998E-2</v>
       </c>
       <c r="M53">
-        <v>0.97021109999999999</v>
+        <v>0.65080879999999997</v>
       </c>
       <c r="N53">
-        <v>1.160454E-2</v>
+        <v>0.17488426000000001</v>
       </c>
       <c r="O53">
-        <v>1.8184349999999998E-2</v>
+        <v>0.17430691000000001</v>
       </c>
       <c r="P53">
-        <v>0.62872649999999997</v>
+        <v>0.44216995999999997</v>
       </c>
       <c r="Q53">
-        <v>0.36812352999999998</v>
+        <v>0.54384220000000005</v>
       </c>
       <c r="R53">
-        <v>3.1499499999999999E-3</v>
+        <v>1.3987879999999999E-2</v>
       </c>
       <c r="S53">
-        <v>0.92717329999999998</v>
+        <v>0.57958304999999999</v>
       </c>
       <c r="T53">
-        <v>7.1370820000000001E-2</v>
+        <v>0.27405536000000003</v>
       </c>
       <c r="U53">
-        <v>1.45586E-3</v>
+        <v>0.14636156</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
@@ -3894,40 +3894,40 @@
         <v>9.47514E-3</v>
       </c>
       <c r="J54">
-        <v>0.62688524000000001</v>
+        <v>0.63750439999999997</v>
       </c>
       <c r="K54">
-        <v>0.34571122999999998</v>
+        <v>0.33775854</v>
       </c>
       <c r="L54">
-        <v>2.7403549999999999E-2</v>
+        <v>2.4737060000000002E-2</v>
       </c>
       <c r="M54">
-        <v>0.25018293000000003</v>
+        <v>0.44337472</v>
       </c>
       <c r="N54">
-        <v>0.67077509999999996</v>
+        <v>0.37268605999999999</v>
       </c>
       <c r="O54">
-        <v>7.9041970000000003E-2</v>
+        <v>0.18393925</v>
       </c>
       <c r="P54">
-        <v>0.90417605999999995</v>
+        <v>0.76756570000000002</v>
       </c>
       <c r="Q54">
-        <v>9.3155139999999997E-2</v>
+        <v>0.21500853</v>
       </c>
       <c r="R54">
-        <v>2.6687799999999999E-3</v>
+        <v>1.7425699999999999E-2</v>
       </c>
       <c r="S54">
-        <v>0.80304264999999997</v>
+        <v>0.58743053999999995</v>
       </c>
       <c r="T54">
-        <v>0.19382384</v>
+        <v>0.26447480000000001</v>
       </c>
       <c r="U54">
-        <v>3.1334800000000001E-3</v>
+        <v>0.14809464999999999</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -3959,40 +3959,40 @@
         <v>0.15566089999999999</v>
       </c>
       <c r="J55">
-        <v>3.6658490000000002E-2</v>
+        <v>3.8308700000000001E-2</v>
       </c>
       <c r="K55">
-        <v>0.91763170000000005</v>
+        <v>0.90962756</v>
       </c>
       <c r="L55">
-        <v>4.5709930000000003E-2</v>
+        <v>5.2063890000000002E-2</v>
       </c>
       <c r="M55">
-        <v>0.37996977999999998</v>
+        <v>0.23814595999999999</v>
       </c>
       <c r="N55">
-        <v>0.54315789999999997</v>
+        <v>0.56598630000000005</v>
       </c>
       <c r="O55">
-        <v>7.6872360000000001E-2</v>
+        <v>0.19586775000000001</v>
       </c>
       <c r="P55">
-        <v>0.69942519999999997</v>
+        <v>0.57860590000000001</v>
       </c>
       <c r="Q55">
-        <v>0.28911822999999998</v>
+        <v>0.38503477000000003</v>
       </c>
       <c r="R55">
-        <v>1.1456589999999999E-2</v>
+        <v>3.6359339999999997E-2</v>
       </c>
       <c r="S55">
-        <v>7.7952160000000006E-2</v>
+        <v>0.22674003000000001</v>
       </c>
       <c r="T55">
-        <v>0.67661420000000005</v>
+        <v>0.57083059999999997</v>
       </c>
       <c r="U55">
-        <v>0.2454336</v>
+        <v>0.20242937999999999</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
@@ -4024,40 +4024,40 @@
         <v>0.11166895</v>
       </c>
       <c r="J56">
-        <v>0.75886509999999996</v>
+        <v>0.68709799999999999</v>
       </c>
       <c r="K56">
-        <v>0.18889934999999999</v>
+        <v>0.21986641000000001</v>
       </c>
       <c r="L56">
-        <v>5.2235589999999998E-2</v>
+        <v>9.3035560000000003E-2</v>
       </c>
       <c r="M56">
-        <v>0.49831170000000002</v>
+        <v>0.43296948000000002</v>
       </c>
       <c r="N56">
-        <v>0.23585313999999999</v>
+        <v>0.25610836999999997</v>
       </c>
       <c r="O56">
-        <v>0.26583522999999998</v>
+        <v>0.31092212000000002</v>
       </c>
       <c r="P56">
-        <v>0.2888618</v>
+        <v>0.37371668000000002</v>
       </c>
       <c r="Q56">
-        <v>0.45668393000000002</v>
+        <v>0.2961685</v>
       </c>
       <c r="R56">
-        <v>0.25445427999999998</v>
+        <v>0.33011479999999999</v>
       </c>
       <c r="S56">
-        <v>0.4966354</v>
+        <v>0.42483514999999999</v>
       </c>
       <c r="T56">
-        <v>0.46694989999999997</v>
+        <v>0.35660589999999998</v>
       </c>
       <c r="U56">
-        <v>3.6414670000000003E-2</v>
+        <v>0.21855896999999999</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
@@ -4089,40 +4089,40 @@
         <v>8.6701669999999995E-2</v>
       </c>
       <c r="J57">
-        <v>5.4346060000000002E-2</v>
+        <v>9.903228E-2</v>
       </c>
       <c r="K57">
-        <v>0.91101840000000001</v>
+        <v>0.860985</v>
       </c>
       <c r="L57">
-        <v>3.4635520000000003E-2</v>
+        <v>3.9982860000000002E-2</v>
       </c>
       <c r="M57">
-        <v>0.10737345</v>
+        <v>0.24035699999999999</v>
       </c>
       <c r="N57">
-        <v>0.7200995</v>
+        <v>0.56093853999999999</v>
       </c>
       <c r="O57">
-        <v>0.17252703</v>
+        <v>0.19870444000000001</v>
       </c>
       <c r="P57">
-        <v>1.7489520000000001E-2</v>
+        <v>8.6476659999999997E-2</v>
       </c>
       <c r="Q57">
-        <v>0.98018780000000005</v>
+        <v>0.89129639999999999</v>
       </c>
       <c r="R57">
-        <v>2.3226700000000002E-3</v>
+        <v>2.2226940000000001E-2</v>
       </c>
       <c r="S57">
-        <v>9.1116799999999998E-2</v>
+        <v>0.22922013999999999</v>
       </c>
       <c r="T57">
-        <v>0.53227716999999997</v>
+        <v>0.46041176</v>
       </c>
       <c r="U57">
-        <v>0.37660605000000003</v>
+        <v>0.31036809999999998</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
@@ -4154,40 +4154,40 @@
         <v>3.7073000000000002E-3</v>
       </c>
       <c r="J58">
-        <v>0.50679039999999997</v>
+        <v>0.55532979999999998</v>
       </c>
       <c r="K58">
-        <v>0.49113852000000002</v>
+        <v>0.43692683999999998</v>
       </c>
       <c r="L58">
-        <v>2.0711200000000001E-3</v>
+        <v>7.7433199999999997E-3</v>
       </c>
       <c r="M58">
-        <v>0.97138599999999997</v>
+        <v>0.65080879999999997</v>
       </c>
       <c r="N58">
-        <v>1.114682E-2</v>
+        <v>0.17488426000000001</v>
       </c>
       <c r="O58">
-        <v>1.7467119999999999E-2</v>
+        <v>0.17430691000000001</v>
       </c>
       <c r="P58">
-        <v>0.61947209999999997</v>
+        <v>0.76533364999999998</v>
       </c>
       <c r="Q58">
-        <v>0.37868144999999998</v>
+        <v>0.22077835000000001</v>
       </c>
       <c r="R58">
-        <v>1.84647E-3</v>
+        <v>1.3887999999999999E-2</v>
       </c>
       <c r="S58">
-        <v>0.99056493999999995</v>
+        <v>0.64643704999999996</v>
       </c>
       <c r="T58">
-        <v>8.2670499999999997E-3</v>
+        <v>0.19305613999999999</v>
       </c>
       <c r="U58">
-        <v>1.1680099999999999E-3</v>
+        <v>0.16050677999999999</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
@@ -4219,40 +4219,40 @@
         <v>1.633099E-2</v>
       </c>
       <c r="J59">
-        <v>9.7660860000000002E-2</v>
+        <v>0.12933844</v>
       </c>
       <c r="K59">
-        <v>0.89800584000000006</v>
+        <v>0.85998182999999995</v>
       </c>
       <c r="L59">
-        <v>4.3332900000000001E-3</v>
+        <v>1.067977E-2</v>
       </c>
       <c r="M59">
-        <v>0.75244652999999995</v>
+        <v>0.43214219999999998</v>
       </c>
       <c r="N59">
-        <v>0.13771378000000001</v>
+        <v>0.37742636000000002</v>
       </c>
       <c r="O59">
-        <v>0.10983966000000001</v>
+        <v>0.19043149000000001</v>
       </c>
       <c r="P59">
-        <v>7.802547E-2</v>
+        <v>0.19466280999999999</v>
       </c>
       <c r="Q59">
-        <v>0.87934239999999997</v>
+        <v>0.70861112999999998</v>
       </c>
       <c r="R59">
-        <v>4.2632139999999999E-2</v>
+        <v>9.6726090000000001E-2</v>
       </c>
       <c r="S59">
-        <v>0.15422875999999999</v>
+        <v>0.25741792000000002</v>
       </c>
       <c r="T59">
-        <v>0.72887650000000004</v>
+        <v>0.50232624999999997</v>
       </c>
       <c r="U59">
-        <v>0.11689471999999999</v>
+        <v>0.24025589</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
@@ -4284,40 +4284,40 @@
         <v>9.7535699999999996E-3</v>
       </c>
       <c r="J60">
-        <v>0.24458884</v>
+        <v>0.30846580000000001</v>
       </c>
       <c r="K60">
-        <v>0.75083864</v>
+        <v>0.67734609999999995</v>
       </c>
       <c r="L60">
-        <v>4.5725899999999996E-3</v>
+        <v>1.418821E-2</v>
       </c>
       <c r="M60">
-        <v>0.66762189999999999</v>
+        <v>0.56053805000000001</v>
       </c>
       <c r="N60">
-        <v>0.27331035999999997</v>
+        <v>0.24833256000000001</v>
       </c>
       <c r="O60">
-        <v>5.9067750000000002E-2</v>
+        <v>0.19112941999999999</v>
       </c>
       <c r="P60">
-        <v>0.92629550000000005</v>
+        <v>0.87928735999999996</v>
       </c>
       <c r="Q60">
-        <v>3.5686629999999997E-2</v>
+        <v>8.4078269999999997E-2</v>
       </c>
       <c r="R60">
-        <v>3.8017809999999999E-2</v>
+        <v>3.6634409999999999E-2</v>
       </c>
       <c r="S60">
-        <v>0.55168660000000003</v>
+        <v>0.52673197000000005</v>
       </c>
       <c r="T60">
-        <v>0.43407016999999998</v>
+        <v>0.29220239999999997</v>
       </c>
       <c r="U60">
-        <v>1.424331E-2</v>
+        <v>0.1810657</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
@@ -4349,40 +4349,40 @@
         <v>6.0527100000000002E-3</v>
       </c>
       <c r="J61">
-        <v>8.744209E-2</v>
+        <v>0.12728818</v>
       </c>
       <c r="K61">
-        <v>0.89312272999999998</v>
+        <v>0.84811029999999998</v>
       </c>
       <c r="L61">
-        <v>1.943516E-2</v>
+        <v>2.460149E-2</v>
       </c>
       <c r="M61">
-        <v>8.1489950000000005E-2</v>
+        <v>0.21762915999999999</v>
       </c>
       <c r="N61">
-        <v>0.85205774999999995</v>
+        <v>0.58324545999999999</v>
       </c>
       <c r="O61">
-        <v>6.6452369999999997E-2</v>
+        <v>0.19912537999999999</v>
       </c>
       <c r="P61">
-        <v>0.10074058</v>
+        <v>0.33769798000000001</v>
       </c>
       <c r="Q61">
-        <v>0.88429080000000004</v>
+        <v>0.6034233</v>
       </c>
       <c r="R61">
-        <v>1.496864E-2</v>
+        <v>5.8878729999999997E-2</v>
       </c>
       <c r="S61">
-        <v>0.26886514</v>
+        <v>0.42277628</v>
       </c>
       <c r="T61">
-        <v>0.72255873999999998</v>
+        <v>0.40801203000000003</v>
       </c>
       <c r="U61">
-        <v>8.5760799999999998E-3</v>
+        <v>0.16921175999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>